<commit_message>
doing homework_1 of DS
</commit_message>
<xml_diff>
--- a/self_practice/news_cafef.xlsx
+++ b/self_practice/news_cafef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\VSCode\DS_project\self_practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E58E8B-F224-4A08-885D-A4D78C471FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B397A64-25D4-477B-8B34-A9DF60533DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>Title</t>
   </si>
@@ -31,6 +31,21 @@
     <t>Summary</t>
   </si>
   <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Hà Nội cho học sinh nghỉ học ngày 6/10</t>
+  </si>
+  <si>
+    <t>2025-10-05T18:24:00</t>
+  </si>
+  <si>
+    <t>Sở GD&amp;ĐT Hà Nội đề nghị các đơn vị cho học sinh nghỉ học ngày mai (6/10) để tránh bão số 11 Matmo.</t>
+  </si>
+  <si>
+    <t>https://cafef.vn/ha-noi-cho-23-trieu-hoc-sinh-nghi-hoc-ngay-6-10-ung-pho-bao-so-11-matmo-188251005182149527.chn</t>
+  </si>
+  <si>
     <t>Không có việc Hoàng Hường vẫn đang làm từ thiện trên Facebook dù đã bị khởi tố, bắt tạm giam</t>
   </si>
   <si>
@@ -40,6 +55,9 @@
     <t>Từ chiều 4/10, người dùng mạng vẫn liên tục thấy nhiều hình ảnh, clip quay lại cảnh bà Hoàng Hường đang đi làm từ thiện ở vùng lũ.</t>
   </si>
   <si>
+    <t>https://cafef.vn/khong-co-viec-hoang-huong-van-dang-lam-tu-thien-tren-facebook-du-da-bi-khoi-to-bat-tam-giam-188251005165823089.chn</t>
+  </si>
+  <si>
     <t>Ông Lê Ngọc Quang được chỉ định giữ chức Bí thư Tỉnh uỷ Quảng Trị</t>
   </si>
   <si>
@@ -49,6 +67,9 @@
     <t>Ông Lê Ngọc Quang được Bộ Chính trị, Ban Bí thư chỉ định giữ chức vụ Bí thư Tỉnh uỷ Quảng Trị nhiệm kỳ 2025 - 2030.</t>
   </si>
   <si>
+    <t>https://cafef.vn/ong-le-ngoc-quang-duoc-chi-dinh-giu-chuc-bi-thu-tinh-uy-quang-tri-188251005165602554.chn</t>
+  </si>
+  <si>
     <t>Bắt tạm giam "Thuỷ Tẹt Bé Nhỏ"</t>
   </si>
   <si>
@@ -58,6 +79,9 @@
     <t>Nông Thị Thu Thủy (Thuỷ Tẹt Bé Nhỏ) đã tạo dựng hình ảnh "trong sáng, nhân hậu" để bớt xén tiền quyên góp từ thiện.</t>
   </si>
   <si>
+    <t>https://cafef.vn/bat-tam-giam-thuy-tet-be-nho-188251005142828335.chn</t>
+  </si>
+  <si>
     <t>Khám xét và bắt tạm giam Giám đốc Bùi Văn Bình</t>
   </si>
   <si>
@@ -67,6 +91,9 @@
     <t>Bùi Văn Bình là Giám đốc Công ty Tân Thuận Phong đã bị Bộ Công an bắt giữ.</t>
   </si>
   <si>
+    <t>https://cafef.vn/kham-xet-va-bat-tam-giam-giam-doc-bui-van-binh-188251005131259582.chn</t>
+  </si>
+  <si>
     <t>Thông tin khẩn về 5 sân bay ảnh hưởng bão Matmo</t>
   </si>
   <si>
@@ -76,6 +103,9 @@
     <t>Trước diễn biến phức tạp của bão Matmo (bão số 11), Cục Hàng không Việt Nam vừa phát văn bản khẩn, yêu cầu các sân bay Vân Đồn, Cát Bi, Nội Bài, Vinh và Thọ Xuân chủ động kiểm tra...</t>
   </si>
   <si>
+    <t>https://cafef.vn/thong-tin-khan-ve-5-san-bay-anh-huong-bao-matmo-188251005131457805.chn</t>
+  </si>
+  <si>
     <t>Bên trong xưởng sản xuất 2,2 triệu bình chữa cháy giả: Công thức pha trộn “tự nghĩ ra”, 54% là bột không có tác dụng dập lửa</t>
   </si>
   <si>
@@ -85,6 +115,9 @@
     <t>Cơ quan CSĐT Công an tỉnh Phú Thọ thi hành quyết định Khởi tố bị can đối với Phan Bạch Thông về tội sản xuất, buôn bán hàng giả.</t>
   </si>
   <si>
+    <t>https://cafef.vn/ben-trong-xuong-san-xuat-22-trieu-binh-chua-chay-gia-cong-thuc-pha-tron-tu-nghi-ra-54-la-bot-khong-co-tac-dung-dap-lua-188251005113331212.chn</t>
+  </si>
+  <si>
     <t>Vụ gây rối tại karaoke Dubai ở Đà Nẵng: Bắt "Xĩn Nghiêm" cùng 3 người</t>
   </si>
   <si>
@@ -94,6 +127,9 @@
     <t>Mâu thuẫn trong lúc mời bia, nam thanh niên ở Đà Nẵng rời đi rồi cùng 3 thanh niên quay lại, mang theo hung khí tấn công nhóm bạn nhậu.</t>
   </si>
   <si>
+    <t>https://cafef.vn/vu-gay-roi-tai-karaoke-dubai-o-da-nang-bat-xin-nghiem-cung-3-nguoi-18825100511362671.chn</t>
+  </si>
+  <si>
     <t>Chủ tịch xã nói gì về việc bí thư xã bị “tố” bỏ lớp bồi dưỡng để chơi Pickleball?</t>
   </si>
   <si>
@@ -103,6 +139,9 @@
     <t>Liên quan vụ việc bí thư xã ở Gia Lai bị phản ánh bỏ lớp bồi dưỡng cán bộ để tham gia giải Pickleball, các cơ quan chức năng đang xác minh, làm rõ.</t>
   </si>
   <si>
+    <t>https://cafef.vn/chu-tich-xa-noi-gi-ve-viec-bi-thu-xa-bi-to-bo-lop-boi-duong-de-choi-pickleball-188251005113845969.chn</t>
+  </si>
+  <si>
     <t>Quảng Ninh cấm biển từ 8h ngày 5/10</t>
   </si>
   <si>
@@ -112,6 +151,9 @@
     <t>Từ 8h ngày 5/10/2025, Sở Nông nghiệp và Môi trường Quảng Ninh thông báo tạm ngừng cấp phép cho các phương tiện thủy ra khơi, tạm dừng hoạt động tham quan, lưu trú trên biển...</t>
   </si>
   <si>
+    <t>https://cafef.vn/quang-ninh-cam-bien-tu-8h-ngay-5-10-188251005103156113.chn</t>
+  </si>
+  <si>
     <t>Bão số 11 tăng cấp, "đi như lướt" trên biển: Khi nào sẽ đổ bộ, ảnh hưởng những vùng nào của Việt Nam?</t>
   </si>
   <si>
@@ -121,6 +163,9 @@
     <t>Trung tâm Dự báo khí tượng thủy văn Quốc gia cho biết cơn bão này có sức phá hoại cực kỳ lớn, sóng biển cực kỳ mạnh.</t>
   </si>
   <si>
+    <t>https://cafef.vn/bao-so-11-tang-cap-di-nhu-luot-tren-bien-khi-nao-se-do-bo-anh-huong-nhung-vung-nao-cua-viet-nam-188251005094305869.chn</t>
+  </si>
+  <si>
     <t>Chủ tịch Hà Nội: Chủ động cho học sinh nghỉ học, người lao động làm việc online ứng phó bão số 11</t>
   </si>
   <si>
@@ -130,6 +175,9 @@
     <t>Hà Nội giao Sở Giáo dục và Đào tạo kiểm tra phương án bảo đảm an toàn cho giáo viên, học sinh, chủ động cho học sinh nghỉ học khi cần. Đồng thời khuyến khích các cơ quan, tổ...</t>
   </si>
   <si>
+    <t>https://cafef.vn/chu-tich-ha-noi-chu-dong-cho-hoc-sinh-nghi-hoc-nguoi-lao-dong-lam-viec-online-ung-pho-bao-so-11-18825100510175321.chn</t>
+  </si>
+  <si>
     <t>Công an bắt quả tang Hoàng Văn Tuyên khi đang livestream</t>
   </si>
   <si>
@@ -139,6 +187,9 @@
     <t>Cơ quan An ninh điều tra phát hiện, bắt quả tang nHoàng Văn Tuyên; Nông Đình Triệu đang thực hiện việc livestream “đổ thạch”.</t>
   </si>
   <si>
+    <t>https://cafef.vn/cong-an-bat-qua-tang-hoang-van-tuyen-khi-dang-livestream-188251005094055791.chn</t>
+  </si>
+  <si>
     <t>Công an cảnh báo khẩn về thông tin "Chính phủ tặng mỗi người dân 1 triệu đồng dịp Tết"</t>
   </si>
   <si>
@@ -148,6 +199,9 @@
     <t>Thông tin "Chính phủ tặng mỗi người dân 1 triệu đồng nhân dịp Tết Nguyên đán" là thông tin chưa được xác thực.</t>
   </si>
   <si>
+    <t>https://cafef.vn/cong-an-canh-bao-khan-ve-thong-tin-chinh-phu-tang-moi-nguoi-dan-1-trieu-dong-dip-tet-188251005083649401.chn</t>
+  </si>
+  <si>
     <t>Hà Nội khuyến khích người dân làm việc online vào thứ Hai ngày 6/10</t>
   </si>
   <si>
@@ -157,6 +211,9 @@
     <t>Hà Nội khuyến khích các cơ quan, tổ chức bố trí cho cán bộ, công chức, viên chức và người lao động làm việc trực tuyến (online) vào Thứ 2 (ngày 6/10).</t>
   </si>
   <si>
+    <t>https://cafef.vn/ha-noi-khuyen-khich-nguoi-dan-lam-viec-online-vao-thu-hai-ngay-6-10-188251005084453025.chn</t>
+  </si>
+  <si>
     <t>Thi hành lệnh khám xét nơi ở của nữ kế toán Phạm Thị Thủy</t>
   </si>
   <si>
@@ -166,6 +223,9 @@
     <t>Đối tượng Phạm Thị Thủy bị khởi tố để điều tra về tội "Mua bán trái phép hóa đơn".</t>
   </si>
   <si>
+    <t>https://cafef.vn/thi-hanh-lenh-kham-xet-noi-o-cua-nu-ke-toan-pham-thi-thuy-188251005083240511.chn</t>
+  </si>
+  <si>
     <t>Bắt tạm giam giám đốc Phan Thế Hoài và em trai Phan Bạch Thông</t>
   </si>
   <si>
@@ -175,6 +235,9 @@
     <t>Công an tỉnh Phú Thọ vừa bắt tạm giam 2 anh em ruột với cáo buộc sản xuất hơn 2 triệu bình chữa cháy giả, thu về hơn 834 tỷ đồng.</t>
   </si>
   <si>
+    <t>https://cafef.vn/bat-tam-giam-giam-doc-phan-the-hoai-va-em-trai-phan-bach-thong-188251005071021839.chn</t>
+  </si>
+  <si>
     <t>Bão số 11 sức gió rất mạnh sắp đổ bộ vào nước ta: Hà Nội và 16 tỉnh, thành đặc biệt chú ý</t>
   </si>
   <si>
@@ -184,6 +247,9 @@
     <t>Cơ quan khí tượng cảnh báo, do ảnh hưởng của hoàn lưu bão rộng, cần đề phòng nguy cơ xảy ra dông, lốc và gió giật mạnh cả trước và trong khi bão đổ bộ.</t>
   </si>
   <si>
+    <t>https://cafef.vn/bao-so-11-suc-gio-rat-manh-sap-do-bo-vao-nuoc-ta-ha-noi-va-16-tinh-thanh-dac-biet-chu-y-188251005071318815.chn</t>
+  </si>
+  <si>
     <t>Bắt tạm giam, khám xét nơi ở của Nguyễn Văn Trình</t>
   </si>
   <si>
@@ -193,6 +259,9 @@
     <t>Nguyễn Văn Trình là đối tượng sử dụng trái phép tài sản của người khác hàng tỷ đồng.</t>
   </si>
   <si>
+    <t>https://cafef.vn/bat-tam-giam-kham-xet-noi-o-cua-nguyen-van-trinh-188251005070837688.chn</t>
+  </si>
+  <si>
     <t>Hà Nội: Cháy phòng giao dịch ngân hàng ở đường Thụy Khuê</t>
   </si>
   <si>
@@ -202,13 +271,7 @@
     <t>Tối 4/10, một vụ hỏa hoạn xảy ra tại trụ sở phòng giao dịch ngân hàng trên đường Thụy Khuê (Hà Nội).</t>
   </si>
   <si>
-    <t>Bộ Công an thông tin về vụ nữ doanh nhân Hoàng Hường bị bắt</t>
-  </si>
-  <si>
-    <t>2025-10-04T20:54:00</t>
-  </si>
-  <si>
-    <t>Ngoài nữ doanh nhân Hoàng Hường, Bộ Công an còn khởi tố, bắt tạm giam nhiều người khác trong hệ sinh thái của bị can này.</t>
+    <t>https://cafef.vn/ha-noi-chay-phong-giao-dich-ngan-hang-o-duong-thuy-khue-188251004213035091.chn</t>
   </si>
 </sst>
 </file>
@@ -571,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A15:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,9 +645,10 @@
     <col min="1" max="1" width="104.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="156.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="141" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,225 +658,288 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="D15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="D17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="D19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="D20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>82</v>
+      </c>
+      <c r="D21" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>